<commit_message>
Add links to software in README
</commit_message>
<xml_diff>
--- a/data/processed/fertilizer_trial_WUR.xlsx
+++ b/data/processed/fertilizer_trial_WUR.xlsx
@@ -1,319 +1,312 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\PPS_R\MiRA\data\processed\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{852052F2-0DFE-458F-BEA4-A4D8D77066AE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="meta" sheetId="2" r:id="rId2"/>
-    <sheet name="variable definitions" sheetId="3" r:id="rId3"/>
+    <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="meta" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="variable definitions" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="95">
-  <si>
-    <t>field_id</t>
-  </si>
-  <si>
-    <t>farm</t>
-  </si>
-  <si>
-    <t>fertilizer</t>
-  </si>
-  <si>
-    <t>yield$tha</t>
-  </si>
-  <si>
-    <t>de Jong</t>
-  </si>
-  <si>
-    <t>SuperDash</t>
-  </si>
-  <si>
-    <t>Miracle</t>
-  </si>
-  <si>
-    <t>Efficientie</t>
-  </si>
-  <si>
-    <t>de Kerk</t>
-  </si>
-  <si>
-    <t>van de Boer</t>
-  </si>
-  <si>
-    <t>field</t>
-  </si>
-  <si>
-    <t>field_name</t>
-  </si>
-  <si>
-    <t>values</t>
-  </si>
-  <si>
-    <t>Data ID</t>
-  </si>
-  <si>
-    <t>data.id</t>
-  </si>
-  <si>
-    <t>Official title of the dataset</t>
-  </si>
-  <si>
-    <t>data.title</t>
-  </si>
-  <si>
-    <t>Meststof proef WUR</t>
-  </si>
-  <si>
-    <t>Project name</t>
-  </si>
-  <si>
-    <t>project.name</t>
-  </si>
-  <si>
-    <t>Meststof Agri Innovatie</t>
-  </si>
-  <si>
-    <t>Description of project</t>
-  </si>
-  <si>
-    <t>project.description</t>
-  </si>
-  <si>
-    <t>Dutch nation-wide fertilizer trial</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>Antoine Longuillaume</t>
-  </si>
-  <si>
-    <t>Author ID(ORCID)</t>
-  </si>
-  <si>
-    <t>orcid</t>
-  </si>
-  <si>
-    <t>Contributor(s)</t>
-  </si>
-  <si>
-    <t>contributors</t>
-  </si>
-  <si>
-    <t>AgriRijnVallei</t>
-  </si>
-  <si>
-    <t>Subject matter of research/Vocabulary</t>
-  </si>
-  <si>
-    <t>subject.research</t>
-  </si>
-  <si>
-    <t>Data origin</t>
-  </si>
-  <si>
-    <t>data.origin</t>
-  </si>
-  <si>
-    <t>Field trial</t>
-  </si>
-  <si>
-    <t>Funder(s) or sponsor(s) of project</t>
-  </si>
-  <si>
-    <t>donor</t>
-  </si>
-  <si>
-    <t>AgriRijnVallei ; NWO</t>
-  </si>
-  <si>
-    <t>creation date (m/d/yyyy)</t>
-  </si>
-  <si>
-    <t>date.creation</t>
-  </si>
-  <si>
-    <t>43784</t>
-  </si>
-  <si>
-    <t>Embargo end date</t>
-  </si>
-  <si>
-    <t>date.embargo</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Citation</t>
-  </si>
-  <si>
-    <t>citation</t>
-  </si>
-  <si>
-    <t>keywords (AGROVOC)</t>
-  </si>
-  <si>
-    <t>keywords.agrovoc</t>
-  </si>
-  <si>
-    <t>Country(ies) covered</t>
-  </si>
-  <si>
-    <t>countries</t>
-  </si>
-  <si>
-    <t>The Netherlands</t>
-  </si>
-  <si>
-    <t>Point longitude coord. in Dec. Degrees</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>Agro-Ecological Zone(s)(FAO) covered</t>
-  </si>
-  <si>
-    <t>aez</t>
-  </si>
-  <si>
-    <t>Years covered by data</t>
-  </si>
-  <si>
-    <t>years</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>Crops covered by data</t>
-  </si>
-  <si>
-    <t>crops</t>
-  </si>
-  <si>
-    <t>Maize</t>
-  </si>
-  <si>
-    <t>Animals covered by data</t>
-  </si>
-  <si>
-    <t>animals</t>
-  </si>
-  <si>
-    <t>Start date of data collection</t>
-  </si>
-  <si>
-    <t>date.collect.start</t>
-  </si>
-  <si>
-    <t>43753</t>
-  </si>
-  <si>
-    <t>End date of data collection</t>
-  </si>
-  <si>
-    <t>date.collect.end</t>
-  </si>
-  <si>
-    <t>43768</t>
-  </si>
-  <si>
-    <t>License (default=CC-BY)</t>
-  </si>
-  <si>
-    <t>licence</t>
-  </si>
-  <si>
-    <t>Permission given by email</t>
-  </si>
-  <si>
-    <t>permission</t>
-  </si>
-  <si>
-    <t>Rights</t>
-  </si>
-  <si>
-    <t>rights</t>
-  </si>
-  <si>
-    <t>Contact email</t>
-  </si>
-  <si>
-    <t>contact.mail</t>
-  </si>
-  <si>
-    <t>antoine.longuillaume@wur.nl</t>
-  </si>
-  <si>
-    <t>workbook</t>
-  </si>
-  <si>
-    <t>sheet</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>definition</t>
-  </si>
-  <si>
-    <t>unique.id</t>
-  </si>
-  <si>
-    <t>personal.information</t>
-  </si>
-  <si>
-    <t>WUR_ferlilizer_trials</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>unique field identifier</t>
-  </si>
-  <si>
-    <t>name of the farm where the experiment was performed</t>
-  </si>
-  <si>
-    <t>type of fertilizer used</t>
-  </si>
-  <si>
-    <t>yield</t>
-  </si>
-  <si>
-    <t>tha</t>
-  </si>
-  <si>
-    <t>maize yield</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+  <si>
+    <t xml:space="preserve">field_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fertilizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yield$tha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de Jong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SuperDash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miracle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficientie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de Kerk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">van de Boer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Official title of the dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meststof proef WUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meststof Agri Innovatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project.description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch nation-wide fertilizer trial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antoine Longuillaume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author ID(ORCID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orcid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributor(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contributors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgriRijnVallei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject matter of research/Vocabulary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subject.research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field trial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funder(s) or sponsor(s) of project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgriRijnVallei ; NWO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creation date (m/d/yyyy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date.creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embargo end date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date.embargo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keywords (AGROVOC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keywords.agrovoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country(ies) covered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point longitude coord. in Dec. Degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agro-Ecological Zone(s)(FAO) covered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years covered by data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crops covered by data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animals covered by data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">animals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start date of data collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date.collect.start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End date of data collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date.collect.end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">License (default=CC-BY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">licence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permission given by email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antoine.longuillaume@wur.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personal.information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WUR_ferlilizer_trials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique field identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name of the farm where the experiment was performed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type of fertilizer used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maize yield</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -349,15 +342,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -639,14 +623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -660,8 +644,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -670,12 +654,12 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D2" t="n">
+        <v>8.3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -684,12 +668,12 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>9.6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -698,9 +682,10 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="D4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -709,12 +694,12 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>7.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -723,12 +708,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>8.4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -737,12 +722,12 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="D7" t="n">
+        <v>8.2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -751,12 +736,12 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="D8" t="n">
+        <v>8.8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -765,12 +750,12 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="D9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -779,12 +764,12 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>7.4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -793,12 +778,12 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="D11" t="n">
+        <v>8.3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -807,12 +792,12 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>10.1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13">
+      <c r="A13" t="n">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -821,12 +806,12 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>10.3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14">
+      <c r="A14" t="n">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -835,12 +820,12 @@
       <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>10.8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15">
+      <c r="A15" t="n">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -849,12 +834,12 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="D15">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="D15" t="n">
+        <v>9.8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -863,12 +848,12 @@
       <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="D16">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="D16" t="n">
+        <v>9.8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -877,12 +862,12 @@
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="n">
         <v>10.9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18">
+      <c r="A18" t="n">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -891,12 +876,12 @@
       <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>12.1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19">
+      <c r="A19" t="n">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -905,12 +890,12 @@
       <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="n">
         <v>11.2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20">
+      <c r="A20" t="n">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -919,12 +904,12 @@
       <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <v>10.9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21">
+      <c r="A21" t="n">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -933,12 +918,12 @@
       <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="n">
         <v>10.1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22">
+      <c r="A22" t="n">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -947,12 +932,12 @@
       <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="n">
         <v>13.2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23">
+      <c r="A23" t="n">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -961,12 +946,12 @@
       <c r="C23" t="s">
         <v>7</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24">
+      <c r="A24" t="n">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -975,12 +960,12 @@
       <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>13.6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25">
+      <c r="A25" t="n">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -989,12 +974,12 @@
       <c r="C25" t="s">
         <v>7</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>13.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26">
+      <c r="A26" t="n">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -1003,12 +988,12 @@
       <c r="C26" t="s">
         <v>7</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>12.6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27">
+      <c r="A27" t="n">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -1017,12 +1002,12 @@
       <c r="C27" t="s">
         <v>7</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>13.4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28">
+      <c r="A28" t="n">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -1031,12 +1016,12 @@
       <c r="C28" t="s">
         <v>7</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="n">
         <v>13.7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29">
+      <c r="A29" t="n">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -1045,12 +1030,12 @@
       <c r="C29" t="s">
         <v>7</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30">
+      <c r="A30" t="n">
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -1059,12 +1044,12 @@
       <c r="C30" t="s">
         <v>7</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="n">
         <v>12.8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31">
+      <c r="A31" t="n">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -1073,12 +1058,12 @@
       <c r="C31" t="s">
         <v>7</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>12.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32">
+      <c r="A32" t="n">
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -1087,12 +1072,12 @@
       <c r="C32" t="s">
         <v>5</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="n">
         <v>8.6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33">
+      <c r="A33" t="n">
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -1101,12 +1086,12 @@
       <c r="C33" t="s">
         <v>5</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="n">
         <v>9.6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="34">
+      <c r="A34" t="n">
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -1115,12 +1100,12 @@
       <c r="C34" t="s">
         <v>5</v>
       </c>
-      <c r="D34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="D34" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -1129,12 +1114,12 @@
       <c r="C35" t="s">
         <v>5</v>
       </c>
-      <c r="D35">
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="D35" t="n">
+        <v>9.2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
         <v>35</v>
       </c>
       <c r="B36" t="s">
@@ -1143,12 +1128,12 @@
       <c r="C36" t="s">
         <v>5</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="n">
         <v>9.9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37">
+      <c r="A37" t="n">
         <v>36</v>
       </c>
       <c r="B37" t="s">
@@ -1157,12 +1142,12 @@
       <c r="C37" t="s">
         <v>5</v>
       </c>
-      <c r="D37">
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="D37" t="n">
+        <v>9.2</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
         <v>37</v>
       </c>
       <c r="B38" t="s">
@@ -1171,12 +1156,12 @@
       <c r="C38" t="s">
         <v>5</v>
       </c>
-      <c r="D38">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="D38" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
         <v>38</v>
       </c>
       <c r="B39" t="s">
@@ -1185,12 +1170,12 @@
       <c r="C39" t="s">
         <v>5</v>
       </c>
-      <c r="D39">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="D39" t="n">
+        <v>8.7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
         <v>39</v>
       </c>
       <c r="B40" t="s">
@@ -1199,12 +1184,12 @@
       <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="n">
         <v>8.4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41">
+      <c r="A41" t="n">
         <v>40</v>
       </c>
       <c r="B41" t="s">
@@ -1213,12 +1198,12 @@
       <c r="C41" t="s">
         <v>5</v>
       </c>
-      <c r="D41">
+      <c r="D41" t="n">
         <v>9.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42">
+      <c r="A42" t="n">
         <v>41</v>
       </c>
       <c r="B42" t="s">
@@ -1227,12 +1212,12 @@
       <c r="C42" t="s">
         <v>6</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="n">
         <v>12.7</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43">
+      <c r="A43" t="n">
         <v>42</v>
       </c>
       <c r="B43" t="s">
@@ -1241,12 +1226,12 @@
       <c r="C43" t="s">
         <v>6</v>
       </c>
-      <c r="D43">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="D43" t="n">
+        <v>10.2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
         <v>43</v>
       </c>
       <c r="B44" t="s">
@@ -1255,12 +1240,12 @@
       <c r="C44" t="s">
         <v>6</v>
       </c>
-      <c r="D44">
+      <c r="D44" t="n">
         <v>10.7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="45">
+      <c r="A45" t="n">
         <v>44</v>
       </c>
       <c r="B45" t="s">
@@ -1269,12 +1254,12 @@
       <c r="C45" t="s">
         <v>6</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="n">
         <v>9.9</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46">
+      <c r="A46" t="n">
         <v>45</v>
       </c>
       <c r="B46" t="s">
@@ -1283,9 +1268,10 @@
       <c r="C46" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="D46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
         <v>46</v>
       </c>
       <c r="B47" t="s">
@@ -1294,12 +1280,12 @@
       <c r="C47" t="s">
         <v>6</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="n">
         <v>10.7</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48">
+      <c r="A48" t="n">
         <v>47</v>
       </c>
       <c r="B48" t="s">
@@ -1308,12 +1294,12 @@
       <c r="C48" t="s">
         <v>6</v>
       </c>
-      <c r="D48">
+      <c r="D48" t="n">
         <v>10.4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49">
+      <c r="A49" t="n">
         <v>48</v>
       </c>
       <c r="B49" t="s">
@@ -1322,12 +1308,12 @@
       <c r="C49" t="s">
         <v>6</v>
       </c>
-      <c r="D49">
+      <c r="D49" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="50">
+      <c r="A50" t="n">
         <v>49</v>
       </c>
       <c r="B50" t="s">
@@ -1336,12 +1322,12 @@
       <c r="C50" t="s">
         <v>6</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="51">
+      <c r="A51" t="n">
         <v>50</v>
       </c>
       <c r="B51" t="s">
@@ -1350,12 +1336,12 @@
       <c r="C51" t="s">
         <v>6</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="52">
+      <c r="A52" t="n">
         <v>51</v>
       </c>
       <c r="B52" t="s">
@@ -1364,12 +1350,12 @@
       <c r="C52" t="s">
         <v>7</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="n">
         <v>12.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="53">
+      <c r="A53" t="n">
         <v>52</v>
       </c>
       <c r="B53" t="s">
@@ -1378,12 +1364,12 @@
       <c r="C53" t="s">
         <v>7</v>
       </c>
-      <c r="D53">
+      <c r="D53" t="n">
         <v>12.6</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="54">
+      <c r="A54" t="n">
         <v>53</v>
       </c>
       <c r="B54" t="s">
@@ -1392,12 +1378,12 @@
       <c r="C54" t="s">
         <v>7</v>
       </c>
-      <c r="D54">
+      <c r="D54" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="55">
+      <c r="A55" t="n">
         <v>54</v>
       </c>
       <c r="B55" t="s">
@@ -1406,12 +1392,12 @@
       <c r="C55" t="s">
         <v>7</v>
       </c>
-      <c r="D55">
+      <c r="D55" t="n">
         <v>12.9</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="56">
+      <c r="A56" t="n">
         <v>55</v>
       </c>
       <c r="B56" t="s">
@@ -1420,12 +1406,12 @@
       <c r="C56" t="s">
         <v>7</v>
       </c>
-      <c r="D56">
+      <c r="D56" t="n">
         <v>12.4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="57">
+      <c r="A57" t="n">
         <v>56</v>
       </c>
       <c r="B57" t="s">
@@ -1434,12 +1420,12 @@
       <c r="C57" t="s">
         <v>7</v>
       </c>
-      <c r="D57">
+      <c r="D57" t="n">
         <v>12.7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="58">
+      <c r="A58" t="n">
         <v>57</v>
       </c>
       <c r="B58" t="s">
@@ -1448,12 +1434,12 @@
       <c r="C58" t="s">
         <v>7</v>
       </c>
-      <c r="D58">
+      <c r="D58" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="59">
+      <c r="A59" t="n">
         <v>58</v>
       </c>
       <c r="B59" t="s">
@@ -1462,12 +1448,12 @@
       <c r="C59" t="s">
         <v>7</v>
       </c>
-      <c r="D59">
+      <c r="D59" t="n">
         <v>12.8</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="60">
+      <c r="A60" t="n">
         <v>59</v>
       </c>
       <c r="B60" t="s">
@@ -1476,12 +1462,12 @@
       <c r="C60" t="s">
         <v>7</v>
       </c>
-      <c r="D60">
+      <c r="D60" t="n">
         <v>12.8</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="61">
+      <c r="A61" t="n">
         <v>60</v>
       </c>
       <c r="B61" t="s">
@@ -1490,12 +1476,12 @@
       <c r="C61" t="s">
         <v>7</v>
       </c>
-      <c r="D61">
+      <c r="D61" t="n">
         <v>13.7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="62">
+      <c r="A62" t="n">
         <v>61</v>
       </c>
       <c r="B62" t="s">
@@ -1504,12 +1490,12 @@
       <c r="C62" t="s">
         <v>5</v>
       </c>
-      <c r="D62">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="D62" t="n">
+        <v>9.3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
         <v>62</v>
       </c>
       <c r="B63" t="s">
@@ -1518,12 +1504,12 @@
       <c r="C63" t="s">
         <v>5</v>
       </c>
-      <c r="D63">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="D63" t="n">
+        <v>8.2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
         <v>63</v>
       </c>
       <c r="B64" t="s">
@@ -1532,12 +1518,12 @@
       <c r="C64" t="s">
         <v>5</v>
       </c>
-      <c r="D64">
+      <c r="D64" t="n">
         <v>9.1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="65">
+      <c r="A65" t="n">
         <v>64</v>
       </c>
       <c r="B65" t="s">
@@ -1546,12 +1532,12 @@
       <c r="C65" t="s">
         <v>5</v>
       </c>
-      <c r="D65">
+      <c r="D65" t="n">
         <v>9.4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row r="66">
+      <c r="A66" t="n">
         <v>65</v>
       </c>
       <c r="B66" t="s">
@@ -1560,12 +1546,12 @@
       <c r="C66" t="s">
         <v>5</v>
       </c>
-      <c r="D66">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="D66" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
         <v>66</v>
       </c>
       <c r="B67" t="s">
@@ -1574,12 +1560,12 @@
       <c r="C67" t="s">
         <v>5</v>
       </c>
-      <c r="D67">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
+      <c r="D67" t="n">
+        <v>8.3</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
         <v>67</v>
       </c>
       <c r="B68" t="s">
@@ -1588,12 +1574,12 @@
       <c r="C68" t="s">
         <v>5</v>
       </c>
-      <c r="D68">
+      <c r="D68" t="n">
         <v>9.9</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
+    <row r="69">
+      <c r="A69" t="n">
         <v>68</v>
       </c>
       <c r="B69" t="s">
@@ -1602,12 +1588,12 @@
       <c r="C69" t="s">
         <v>5</v>
       </c>
-      <c r="D69">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="D69" t="n">
+        <v>8.7</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
         <v>69</v>
       </c>
       <c r="B70" t="s">
@@ -1616,12 +1602,12 @@
       <c r="C70" t="s">
         <v>5</v>
       </c>
-      <c r="D70">
+      <c r="D70" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
+    <row r="71">
+      <c r="A71" t="n">
         <v>70</v>
       </c>
       <c r="B71" t="s">
@@ -1630,9 +1616,10 @@
       <c r="C71" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
+      <c r="D71"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
         <v>71</v>
       </c>
       <c r="B72" t="s">
@@ -1641,12 +1628,12 @@
       <c r="C72" t="s">
         <v>6</v>
       </c>
-      <c r="D72">
+      <c r="D72" t="n">
         <v>10.7</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
+    <row r="73">
+      <c r="A73" t="n">
         <v>72</v>
       </c>
       <c r="B73" t="s">
@@ -1655,12 +1642,12 @@
       <c r="C73" t="s">
         <v>6</v>
       </c>
-      <c r="D73">
+      <c r="D73" t="n">
         <v>10.5</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
+    <row r="74">
+      <c r="A74" t="n">
         <v>73</v>
       </c>
       <c r="B74" t="s">
@@ -1669,12 +1656,12 @@
       <c r="C74" t="s">
         <v>6</v>
       </c>
-      <c r="D74">
+      <c r="D74" t="n">
         <v>10.3</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row r="75">
+      <c r="A75" t="n">
         <v>74</v>
       </c>
       <c r="B75" t="s">
@@ -1683,12 +1670,12 @@
       <c r="C75" t="s">
         <v>6</v>
       </c>
-      <c r="D75">
+      <c r="D75" t="n">
         <v>11.7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row r="76">
+      <c r="A76" t="n">
         <v>75</v>
       </c>
       <c r="B76" t="s">
@@ -1697,12 +1684,12 @@
       <c r="C76" t="s">
         <v>6</v>
       </c>
-      <c r="D76">
+      <c r="D76" t="n">
         <v>10.3</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row r="77">
+      <c r="A77" t="n">
         <v>76</v>
       </c>
       <c r="B77" t="s">
@@ -1711,12 +1698,12 @@
       <c r="C77" t="s">
         <v>6</v>
       </c>
-      <c r="D77">
+      <c r="D77" t="n">
         <v>10.8</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
+    <row r="78">
+      <c r="A78" t="n">
         <v>77</v>
       </c>
       <c r="B78" t="s">
@@ -1725,12 +1712,12 @@
       <c r="C78" t="s">
         <v>6</v>
       </c>
-      <c r="D78">
+      <c r="D78" t="n">
         <v>11.5</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
+    <row r="79">
+      <c r="A79" t="n">
         <v>78</v>
       </c>
       <c r="B79" t="s">
@@ -1739,12 +1726,12 @@
       <c r="C79" t="s">
         <v>6</v>
       </c>
-      <c r="D79">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
+      <c r="D79" t="n">
+        <v>9.3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
         <v>79</v>
       </c>
       <c r="B80" t="s">
@@ -1753,12 +1740,12 @@
       <c r="C80" t="s">
         <v>6</v>
       </c>
-      <c r="D80">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
+      <c r="D80" t="n">
+        <v>10.2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
         <v>80</v>
       </c>
       <c r="B81" t="s">
@@ -1767,12 +1754,12 @@
       <c r="C81" t="s">
         <v>6</v>
       </c>
-      <c r="D81">
+      <c r="D81" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
+    <row r="82">
+      <c r="A82" t="n">
         <v>81</v>
       </c>
       <c r="B82" t="s">
@@ -1781,12 +1768,12 @@
       <c r="C82" t="s">
         <v>7</v>
       </c>
-      <c r="D82">
+      <c r="D82" t="n">
         <v>13.1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
+    <row r="83">
+      <c r="A83" t="n">
         <v>82</v>
       </c>
       <c r="B83" t="s">
@@ -1795,12 +1782,12 @@
       <c r="C83" t="s">
         <v>7</v>
       </c>
-      <c r="D83">
+      <c r="D83" t="n">
         <v>12.7</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84">
+    <row r="84">
+      <c r="A84" t="n">
         <v>83</v>
       </c>
       <c r="B84" t="s">
@@ -1809,12 +1796,12 @@
       <c r="C84" t="s">
         <v>7</v>
       </c>
-      <c r="D84">
+      <c r="D84" t="n">
         <v>13.6</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row r="85">
+      <c r="A85" t="n">
         <v>84</v>
       </c>
       <c r="B85" t="s">
@@ -1823,12 +1810,12 @@
       <c r="C85" t="s">
         <v>7</v>
       </c>
-      <c r="D85">
+      <c r="D85" t="n">
         <v>13.3</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86">
+    <row r="86">
+      <c r="A86" t="n">
         <v>85</v>
       </c>
       <c r="B86" t="s">
@@ -1837,12 +1824,12 @@
       <c r="C86" t="s">
         <v>7</v>
       </c>
-      <c r="D86">
+      <c r="D86" t="n">
         <v>11.7</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87">
+    <row r="87">
+      <c r="A87" t="n">
         <v>86</v>
       </c>
       <c r="B87" t="s">
@@ -1851,12 +1838,12 @@
       <c r="C87" t="s">
         <v>7</v>
       </c>
-      <c r="D87">
+      <c r="D87" t="n">
         <v>14.2</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88">
+    <row r="88">
+      <c r="A88" t="n">
         <v>87</v>
       </c>
       <c r="B88" t="s">
@@ -1865,9 +1852,10 @@
       <c r="C88" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="D88"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
         <v>88</v>
       </c>
       <c r="B89" t="s">
@@ -1876,12 +1864,12 @@
       <c r="C89" t="s">
         <v>7</v>
       </c>
-      <c r="D89">
+      <c r="D89" t="n">
         <v>12.8</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
+    <row r="90">
+      <c r="A90" t="n">
         <v>89</v>
       </c>
       <c r="B90" t="s">
@@ -1890,12 +1878,12 @@
       <c r="C90" t="s">
         <v>7</v>
       </c>
-      <c r="D90">
+      <c r="D90" t="n">
         <v>12.5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
+    <row r="91">
+      <c r="A91" t="n">
         <v>90</v>
       </c>
       <c r="B91" t="s">
@@ -1904,32 +1892,25 @@
       <c r="C91" t="s">
         <v>7</v>
       </c>
-      <c r="D91">
+      <c r="D91" t="n">
         <v>13.6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1940,15 +1921,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1959,7 +1941,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1970,7 +1952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1981,7 +1963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1992,15 +1974,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7"/>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2011,15 +1994,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9"/>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -2030,7 +2014,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2041,7 +2025,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2052,7 +2036,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2063,23 +2047,25 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" t="s">
         <v>46</v>
       </c>
       <c r="B14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14"/>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15"/>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2090,23 +2076,25 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17"/>
+    </row>
+    <row r="18">
       <c r="A18" t="s">
         <v>55</v>
       </c>
       <c r="B18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18"/>
+    </row>
+    <row r="19">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -2117,7 +2105,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2128,7 +2116,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -2139,7 +2127,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -2150,7 +2138,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -2161,15 +2149,16 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" t="s">
         <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24"/>
+    </row>
+    <row r="25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2180,15 +2169,16 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" t="s">
         <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26"/>
+    </row>
+    <row r="27">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -2201,19 +2191,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2236,7 +2226,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -2246,17 +2236,18 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
+      <c r="D2"/>
       <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -2266,17 +2257,18 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
+      <c r="D3"/>
       <c r="E3" t="s">
         <v>90</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -2286,17 +2278,18 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
+      <c r="D4"/>
       <c r="E4" t="s">
         <v>91</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -2312,15 +2305,15 @@
       <c r="E5" t="s">
         <v>94</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>